<commit_message>
Added Normalization Files & Earthquake Project
</commit_message>
<xml_diff>
--- a/Normalization Explanation/Normalization 1NF.xlsx
+++ b/Normalization Explanation/Normalization 1NF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammi\Documents\GitHub\CSCI1320-Public-Repo\CSCI1320-PublicRepo\Normalization Explanation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416774FC-C842-479F-96E9-5BA069139B0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D202017-DB3D-4CC9-90D8-BF3EF7AD82FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="-24420" windowWidth="19524" windowHeight="12840" xr2:uid="{2E7926EF-81B9-45D2-A46B-2635B5BE71DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{2E7926EF-81B9-45D2-A46B-2635B5BE71DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Normalization" sheetId="3" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="74">
   <si>
     <t>Cust_ID</t>
   </si>
   <si>
-    <t>Cust_Nmae</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>Product</t>
   </si>
   <si>
-    <t>Samus Aran</t>
-  </si>
-  <si>
     <t>555-1212</t>
   </si>
   <si>
@@ -249,6 +243,41 @@
   </si>
   <si>
     <t>Mnth_Sal</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>Cust_Name</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
+    <t>Product3</t>
   </si>
 </sst>
 </file>
@@ -547,50 +576,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -608,22 +607,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -634,15 +666,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -960,74 +994,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62FC022-5BF4-4DB3-B8E8-7F0F959976D5}">
   <dimension ref="B1:J15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="108.42578125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="108.42578125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="31"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+    </row>
+    <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+    <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J15" s="21"/>
+      <c r="J15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1041,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C8B10A-09E9-40F1-97BB-0983B08F6909}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView showGridLines="0" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,64 +1087,64 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="29"/>
+        <v>32</v>
+      </c>
+      <c r="C7" s="22"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="29"/>
+        <v>33</v>
+      </c>
+      <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="29"/>
+        <v>34</v>
+      </c>
+      <c r="C9" s="22"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="26" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="28" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1125,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBB1212-E03E-48DD-A4C2-3E7CA559F167}">
   <dimension ref="B3:K55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,85 +1169,85 @@
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="21" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="11" customWidth="1"/>
     <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>10</v>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="22" t="s">
+      <c r="F5" s="24"/>
+      <c r="G5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="23" t="s">
+      <c r="I6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
+    </row>
+    <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="11">
-        <v>5555078</v>
-      </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="C7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D8" s="1"/>
@@ -1229,307 +1263,307 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="E14" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="F14" s="28"/>
+      <c r="G14" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="22" t="s">
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="6">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="9">
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="C16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="9">
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="19" t="s">
+      <c r="C17" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="31"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="9">
-        <v>1</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="9">
-        <v>2</v>
-      </c>
-      <c r="C18" s="8" t="s">
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="33"/>
+      <c r="G25" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" s="6">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D25" s="18" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="7">
         <v>2</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B26" s="9">
-        <v>1</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="C27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="11">
-        <v>2</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="23" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D42" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="J42" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K42" s="23"/>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D42" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="J42" s="24" t="s">
+      <c r="G43" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="J43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K42" s="24"/>
-    </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D43" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="7" t="s">
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D44" s="7">
+        <v>1</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H44" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="J44" s="19">
+        <v>1</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D45" s="7">
+        <v>2</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G43" s="22" t="s">
+      <c r="F45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J45" s="19">
         <v>2</v>
       </c>
-      <c r="H43" s="8"/>
-      <c r="J43" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K43" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D44" s="8">
-        <v>1</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G44" s="9" t="s">
+      <c r="K45" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H44" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J44" s="8">
-        <v>1</v>
-      </c>
-      <c r="K44" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D45" s="8">
-        <v>2</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J45" s="8">
-        <v>2</v>
-      </c>
-      <c r="K45" s="8" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="J46" s="8">
+      <c r="J46" s="19">
         <v>3</v>
       </c>
-      <c r="K46" s="8" t="s">
-        <v>9</v>
+      <c r="K46" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H49" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H50" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I50" s="8"/>
+      <c r="H50" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I50" s="5"/>
     </row>
     <row r="51" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H51" s="7" t="s">
+      <c r="H51" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I51" s="7" t="s">
-        <v>28</v>
+      <c r="I51" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H52" s="8">
+      <c r="H52" s="7">
         <v>1</v>
       </c>
-      <c r="I52" s="8">
+      <c r="I52" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H53" s="8">
+      <c r="H53" s="7">
         <v>1</v>
       </c>
-      <c r="I53" s="8">
+      <c r="I53" s="7">
         <v>2</v>
       </c>
     </row>
     <row r="54" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H54" s="8">
+      <c r="H54" s="7">
         <v>1</v>
       </c>
-      <c r="I54" s="8">
+      <c r="I54" s="7">
         <v>3</v>
       </c>
     </row>
     <row r="55" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H55" s="8">
+      <c r="H55" s="7">
         <v>2</v>
       </c>
-      <c r="I55" s="8">
+      <c r="I55" s="7">
         <v>2</v>
       </c>
     </row>
@@ -1550,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20DEAD4-BF3A-436A-ACBC-F2C616285B48}">
   <dimension ref="C3:I41"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,232 +1597,232 @@
   <sheetData>
     <row r="3" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="8" t="s">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="8" t="s">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="8" t="s">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="8" t="s">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="8" t="s">
-        <v>22</v>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="36" t="s">
+      <c r="D22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="7" t="s">
+      <c r="G22" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="7" t="s">
+      <c r="H22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="I22" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="6">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="9">
-        <v>1</v>
-      </c>
-      <c r="D23" s="8" t="s">
+      <c r="F23" s="5">
+        <v>2500</v>
+      </c>
+      <c r="G23" s="5">
+        <v>2500</v>
+      </c>
+      <c r="H23" s="5">
+        <v>2500</v>
+      </c>
+      <c r="I23" s="35"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" s="6">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E24" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="8">
-        <v>2500</v>
-      </c>
-      <c r="G23" s="8">
-        <v>2500</v>
-      </c>
-      <c r="H23" s="8">
-        <v>2500</v>
-      </c>
-      <c r="I23" s="34"/>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="9">
-        <v>2</v>
-      </c>
-      <c r="D24" s="8" t="s">
+      <c r="F24" s="5">
+        <v>3000</v>
+      </c>
+      <c r="G24" s="5">
+        <v>3000</v>
+      </c>
+      <c r="H24" s="5">
+        <v>3000</v>
+      </c>
+      <c r="I24" s="35"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="6">
+        <v>3</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E25" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F24" s="8">
-        <v>3000</v>
-      </c>
-      <c r="G24" s="8">
-        <v>3000</v>
-      </c>
-      <c r="H24" s="8">
-        <v>3000</v>
-      </c>
-      <c r="I24" s="34"/>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="9">
-        <v>3</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="8">
+      <c r="F25" s="5">
         <v>1800</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="5">
         <v>1800</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="5">
         <v>1800</v>
       </c>
-      <c r="I25" s="35"/>
+      <c r="I25" s="36"/>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G30" s="3"/>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="39"/>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="39"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="40"/>
-    </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="F38" s="37" t="s">
-        <v>70</v>
-      </c>
-      <c r="G38" s="41" t="s">
-        <v>22</v>
+      <c r="E38" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="40" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="9">
+      <c r="C39" s="6">
         <v>1</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F39" s="5">
+        <v>2500</v>
+      </c>
+      <c r="G39" s="40"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="6">
+        <v>2</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="E40" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="F39" s="8">
-        <v>2500</v>
-      </c>
-      <c r="G39" s="41"/>
-    </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="9">
-        <v>2</v>
-      </c>
-      <c r="D40" s="8" t="s">
+      <c r="F40" s="5">
+        <v>3000</v>
+      </c>
+      <c r="G40" s="40"/>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="6">
+        <v>3</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E41" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F40" s="8">
-        <v>3000</v>
-      </c>
-      <c r="G40" s="41"/>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="9">
-        <v>3</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F41" s="8">
+      <c r="F41" s="5">
         <v>1800</v>
       </c>
-      <c r="G41" s="41"/>
+      <c r="G41" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>